<commit_message>
"Get Text activity title adjustments
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\P3 Sales\ScrapeJobPostData\CareerBuilderWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF68E279-9B69-41BB-8465-C21FAA644B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8888D873-6D29-410F-B1FB-0DE8E2213C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
   </bookViews>
   <sheets>
     <sheet name="CareerBuilder" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Job Title</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Job Type</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer</t>
+  </si>
+  <si>
+    <t>Property Matrix</t>
   </si>
 </sst>
 </file>
@@ -398,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB20DF4A-498B-4C2C-BEDF-FEE00E3CB96C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,6 +432,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Got companyName, jobLocation and jobType data
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <x:si>
     <x:t>Job Title</x:t>
   </x:si>
@@ -92,6 +92,36 @@
   </x:si>
   <x:si>
     <x:t>Property Matrix</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Virginia Beach, VA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dallas, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>New York, NY</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Full-Time/Part-Time</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Minneapolis, MN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Milwaukee, WI</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Reston, VA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry Level Remote Home</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fayetteville, NC, NC</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -631,6 +661,727 @@
         <x:v>18</x:v>
       </x:c>
     </x:row>
+    <x:row r="12" spans="1:4">
+      <x:c r="A12" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B12" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C12" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D12" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:4">
+      <x:c r="A13" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B13" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C13" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D13" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:4">
+      <x:c r="A14" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D14" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:4">
+      <x:c r="A15" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D15" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:4">
+      <x:c r="A16" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D16" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:4">
+      <x:c r="A17" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B17" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C17" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D17" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:4">
+      <x:c r="A18" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D18" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:4">
+      <x:c r="A19" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D19" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:4">
+      <x:c r="A20" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B20" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C20" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D20" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:4">
+      <x:c r="A21" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B21" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C21" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D21" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B22" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C22" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D22" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B23" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C23" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D23" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D24" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="25" spans="1:4">
+      <x:c r="A25" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D25" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D26" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B27" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C27" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D27" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D28" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D29" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B30" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C30" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D30" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B31" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C31" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D31" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B32" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C32" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D32" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B33" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C33" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D33" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="34" spans="1:4">
+      <x:c r="A34" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B34" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C34" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D34" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="35" spans="1:4">
+      <x:c r="A35" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B35" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C35" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D35" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="36" spans="1:4">
+      <x:c r="A36" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B36" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C36" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D36" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="37" spans="1:4">
+      <x:c r="A37" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B37" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C37" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D37" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="38" spans="1:4">
+      <x:c r="A38" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B38" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C38" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D38" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="39" spans="1:4">
+      <x:c r="A39" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B39" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C39" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D39" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="40" spans="1:4">
+      <x:c r="A40" s="2" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B40" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C40" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="D40" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="41" spans="1:4">
+      <x:c r="A41" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B41" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C41" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="D41" s="2" t="s">
+        <x:v>18</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:4">
+      <x:c r="A42" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B42" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C42" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D42" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="43" spans="1:4">
+      <x:c r="A43" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B43" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C43" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D43" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="44" spans="1:4">
+      <x:c r="A44" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B44" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C44" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D44" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="45" spans="1:4">
+      <x:c r="A45" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B45" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C45" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D45" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="46" spans="1:4">
+      <x:c r="A46" s="2" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B46" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C46" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D46" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="47" spans="1:4">
+      <x:c r="A47" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B47" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C47" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D47" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="48" spans="1:4">
+      <x:c r="A48" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B48" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C48" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D48" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="49" spans="1:4">
+      <x:c r="A49" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B49" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C49" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D49" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="50" spans="1:4">
+      <x:c r="A50" s="2" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B50" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C50" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D50" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="51" spans="1:4">
+      <x:c r="A51" s="2" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B51" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C51" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="D51" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="52" spans="1:4">
+      <x:c r="A52" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B52" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C52" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D52" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="53" spans="1:4">
+      <x:c r="A53" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B53" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C53" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D53" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="54" spans="1:4">
+      <x:c r="A54" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B54" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C54" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D54" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="55" spans="1:4">
+      <x:c r="A55" s="2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B55" s="2" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C55" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D55" s="2" t="s"/>
+    </x:row>
+    <x:row r="56" spans="1:4">
+      <x:c r="A56" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B56" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C56" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D56" s="2" t="s"/>
+    </x:row>
+    <x:row r="57" spans="1:4">
+      <x:c r="A57" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B57" s="2" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C57" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D57" s="2" t="s"/>
+    </x:row>
+    <x:row r="58" spans="1:4">
+      <x:c r="A58" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B58" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C58" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D58" s="2" t="s"/>
+    </x:row>
+    <x:row r="59" spans="1:4">
+      <x:c r="A59" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B59" s="2" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C59" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D59" s="2" t="s"/>
+    </x:row>
+    <x:row r="60" spans="1:4">
+      <x:c r="A60" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B60" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C60" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D60" s="2" t="s"/>
+    </x:row>
+    <x:row r="61" spans="1:4">
+      <x:c r="A61" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B61" s="2" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="C61" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D61" s="2" t="s"/>
+    </x:row>
+    <x:row r="62" spans="1:4">
+      <x:c r="A62" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B62" s="2" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C62" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D62" s="2" t="s"/>
+    </x:row>
+    <x:row r="63" spans="1:4">
+      <x:c r="A63" s="2" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B63" s="2" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C63" s="2" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="D63" s="2" t="s"/>
+    </x:row>
+    <x:row r="64" spans="1:4">
+      <x:c r="A64" s="2" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B64" s="2" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C64" s="2" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Robot now scrapes Company Size (if available).
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\P3 Sales\P3SalesAutomationSuite\ScrapeJobPostData\CareerBuilderWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E53093-B185-4599-9FBD-0138BC328FE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33319D21-49DC-4FA1-92B6-333C6BB989AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
   </bookViews>
   <sheets>
     <sheet name="CareerBuilder" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>JobTitle</t>
   </si>
@@ -48,6 +48,12 @@
     <t>JobType</t>
   </si>
   <si>
+    <t>CompanySize</t>
+  </si>
+  <si>
+    <t>DatePosted</t>
+  </si>
+  <si>
     <t>Entry-Level Developer - required to work in office</t>
   </si>
   <si>
@@ -58,14 +64,103 @@
   </si>
   <si>
     <t>Full Time</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Entry-level Healthcare Digital Technology Developer</t>
+  </si>
+  <si>
+    <t>Cognizant Technology</t>
+  </si>
+  <si>
+    <t>Dallas, TX</t>
+  </si>
+  <si>
+    <t>Entry-level EAS Digital Technology Developer</t>
+  </si>
+  <si>
+    <t>Entry Level SQL Developer</t>
+  </si>
+  <si>
+    <t>HAWAII MAINLAND ADMINISTRATORS L</t>
+  </si>
+  <si>
+    <t>Tempe, AZ</t>
+  </si>
+  <si>
+    <t>Entry-Level .NET Developer / Application Support</t>
+  </si>
+  <si>
+    <t>Medline Industries, Inc.</t>
+  </si>
+  <si>
+    <t>Mundelein, IL</t>
+  </si>
+  <si>
+    <t>Entry Level Unreal Engine C++ Developer</t>
+  </si>
+  <si>
+    <t>Opex</t>
+  </si>
+  <si>
+    <t>Moorestown, NJ</t>
+  </si>
+  <si>
+    <t>Java Developer - Recent Grads - Entry Level Positions</t>
+  </si>
+  <si>
+    <t>Cogent Infotech.</t>
+  </si>
+  <si>
+    <t>Work From Home</t>
+  </si>
+  <si>
+    <t>Mid to Entry Level Software Developer</t>
+  </si>
+  <si>
+    <t>Robert Half</t>
+  </si>
+  <si>
+    <t>Deer Park, TX</t>
+  </si>
+  <si>
+    <t>Developer, Entry Level</t>
+  </si>
+  <si>
+    <t>Sentinel Technologies Inc.</t>
+  </si>
+  <si>
+    <t>Downers Grove, IL</t>
+  </si>
+  <si>
+    <t>Jr Web Developer (Entry Level)</t>
+  </si>
+  <si>
+    <t>Planned Systems International, Inc.</t>
+  </si>
+  <si>
+    <t>Washington, DC</t>
+  </si>
+  <si>
+    <t>Contractor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,9 +188,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,49 +506,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB20DF4A-498B-4C2C-BEDF-FEE00E3CB96C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="79.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Unique Jobs & Company Size.
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\P3 Sales\P3SalesAutomationSuite\ScrapeJobPostData\CareerBuilderWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33319D21-49DC-4FA1-92B6-333C6BB989AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDAD95E2-02B1-4DBD-B8BD-96262FC2467B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
   </bookViews>
   <sheets>
     <sheet name="CareerBuilder" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>JobTitle</t>
   </si>
@@ -51,9 +51,6 @@
     <t>CompanySize</t>
   </si>
   <si>
-    <t>DatePosted</t>
-  </si>
-  <si>
     <t>Entry-Level Developer - required to work in office</t>
   </si>
   <si>
@@ -81,70 +78,55 @@
     <t>Entry-level EAS Digital Technology Developer</t>
   </si>
   <si>
-    <t>Entry Level SQL Developer</t>
-  </si>
-  <si>
-    <t>HAWAII MAINLAND ADMINISTRATORS L</t>
-  </si>
-  <si>
-    <t>Tempe, AZ</t>
-  </si>
-  <si>
-    <t>Entry-Level .NET Developer / Application Support</t>
-  </si>
-  <si>
-    <t>Medline Industries, Inc.</t>
-  </si>
-  <si>
-    <t>Mundelein, IL</t>
-  </si>
-  <si>
-    <t>Entry Level Unreal Engine C++ Developer</t>
-  </si>
-  <si>
-    <t>Opex</t>
-  </si>
-  <si>
-    <t>Moorestown, NJ</t>
-  </si>
-  <si>
-    <t>Java Developer - Recent Grads - Entry Level Positions</t>
-  </si>
-  <si>
-    <t>Cogent Infotech.</t>
-  </si>
-  <si>
-    <t>Work From Home</t>
-  </si>
-  <si>
-    <t>Mid to Entry Level Software Developer</t>
-  </si>
-  <si>
-    <t>Robert Half</t>
-  </si>
-  <si>
-    <t>Deer Park, TX</t>
-  </si>
-  <si>
-    <t>Developer, Entry Level</t>
-  </si>
-  <si>
-    <t>Sentinel Technologies Inc.</t>
-  </si>
-  <si>
-    <t>Downers Grove, IL</t>
-  </si>
-  <si>
-    <t>Jr Web Developer (Entry Level)</t>
-  </si>
-  <si>
-    <t>Planned Systems International, Inc.</t>
-  </si>
-  <si>
-    <t>Washington, DC</t>
-  </si>
-  <si>
-    <t>Contractor</t>
+    <t>Work From Home Entry Level Data Entry Associate</t>
+  </si>
+  <si>
+    <t>Level Up Entry</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA, PA</t>
+  </si>
+  <si>
+    <t>Full-Time/Part-Time</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer - Dev10 Technology Development Program - NY</t>
+  </si>
+  <si>
+    <t>Genesis10</t>
+  </si>
+  <si>
+    <t>New York, NY</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer - Dev10 Technology Development Program - WI</t>
+  </si>
+  <si>
+    <t>Milwaukee, WI</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer - Dev10 Technology Development Program - MN</t>
+  </si>
+  <si>
+    <t>Minneapolis, MN</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer - Dev10 Technology Development Program - .NET - TX</t>
+  </si>
+  <si>
+    <t>Entry Level Software Developer - Dev10 Technology Development Program - .NET - MN</t>
+  </si>
+  <si>
+    <t>Software Developer - Entry Level</t>
+  </si>
+  <si>
+    <t>Revature</t>
+  </si>
+  <si>
+    <t>Reston, VA</t>
+  </si>
+  <si>
+    <t>DaysPostedAgo</t>
   </si>
 </sst>
 </file>
@@ -509,7 +491,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,177 +520,177 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added function to write date posted ago/added try-catch blocks to some get text activities
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <x:si>
     <x:t>JobTitle</x:t>
   </x:si>
@@ -70,6 +70,9 @@
     <x:t>N/A</x:t>
   </x:si>
   <x:si>
+    <x:t>16 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Work From Home Entry Level Data Entry Associate</x:t>
   </x:si>
   <x:si>
@@ -82,6 +85,9 @@
     <x:t>Full-Time/Part-Time</x:t>
   </x:si>
   <x:si>
+    <x:t>5 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry-level Healthcare Digital Technology Developer</x:t>
   </x:si>
   <x:si>
@@ -91,6 +97,9 @@
     <x:t>Dallas, TX</x:t>
   </x:si>
   <x:si>
+    <x:t>20 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry Level Software Developer - Dev10 Technology Development Program - NY</x:t>
   </x:si>
   <x:si>
@@ -100,21 +109,33 @@
     <x:t>New York, NY</x:t>
   </x:si>
   <x:si>
+    <x:t>28 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry Level Software Developer - Dev10 Technology Development Program - WI</x:t>
   </x:si>
   <x:si>
     <x:t>Milwaukee, WI</x:t>
   </x:si>
   <x:si>
+    <x:t>Today</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry Level Software Developer - Dev10 Technology Development Program - MN</x:t>
   </x:si>
   <x:si>
     <x:t>Minneapolis, MN</x:t>
   </x:si>
   <x:si>
+    <x:t>7 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry-level EAS Digital Technology Developer</x:t>
   </x:si>
   <x:si>
+    <x:t>11 days ago</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry Level Software Developer - Dev10 Technology Development Program - .NET - TX</x:t>
   </x:si>
   <x:si>
@@ -128,6 +149,63 @@
   </x:si>
   <x:si>
     <x:t>Reston, VA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21 days ago</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry Level SQL Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>HAWAII MAINLAND ADMINISTRATORS L</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Tempe, AZ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry-Level .NET Developer / Application Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Medline Industries, Inc.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Mundelein, IL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry Level Unreal Engine C++ Developer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Opex</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Moorestown, NJ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry Level Marketing</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DFW Brands</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Entry Level Engineer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Prokatchers LLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Irving, TX</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Contractor</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Facilities Engineer - Electrical - Entry/Experienced Level (NSAW and NSAH)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>National Security Agency (NSA)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fort Meade, MD</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -566,152 +644,179 @@
       <x:c r="E2" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
+      <x:c r="F2" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A3" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B3" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C3" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D3" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E3" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F3" s="3" t="s">
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A4" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B4" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C4" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D4" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E4" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F4" s="3" t="s">
+        <x:v>20</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A5" s="3" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B5" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C5" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D5" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E5" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F5" s="3" t="s">
+        <x:v>24</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A6" s="3" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B6" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C6" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E6" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F6" s="3" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A7" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B7" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C7" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D7" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E7" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F7" s="3" t="s">
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A8" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B8" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C8" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D8" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E8" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F8" s="3" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A9" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B9" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C9" s="3" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="C9" s="3" t="s">
-        <x:v>17</x:v>
-      </x:c>
       <x:c r="D9" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E9" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F9" s="3" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A10" s="3" t="s">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B10" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C10" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D10" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E10" s="3" t="s">
         <x:v>10</x:v>
+      </x:c>
+      <x:c r="F10" s="3" t="s">
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A11" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B11" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C11" s="3" t="s">
-        <x:v>30</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D11" s="3" t="s">
         <x:v>9</x:v>
@@ -719,7 +824,9 @@
       <x:c r="E11" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="F11" s="3" t="s"/>
+      <x:c r="F11" s="3" t="s">
+        <x:v>38</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:6">
       <x:c r="A12" s="3" t="s">
@@ -741,16 +848,16 @@
     </x:row>
     <x:row r="13" spans="1:6">
       <x:c r="A13" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B13" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C13" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D13" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E13" s="3" t="s">
         <x:v>10</x:v>
@@ -795,16 +902,16 @@
     </x:row>
     <x:row r="16" spans="1:6">
       <x:c r="A16" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B16" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C16" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D16" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E16" s="3" t="s">
         <x:v>10</x:v>
@@ -813,13 +920,13 @@
     </x:row>
     <x:row r="17" spans="1:6">
       <x:c r="A17" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B17" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C17" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D17" s="3" t="s">
         <x:v>9</x:v>
@@ -849,16 +956,16 @@
     </x:row>
     <x:row r="19" spans="1:6">
       <x:c r="A19" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B19" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C19" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D19" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E19" s="3" t="s">
         <x:v>10</x:v>
@@ -867,13 +974,13 @@
     </x:row>
     <x:row r="20" spans="1:6">
       <x:c r="A20" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B20" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C20" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D20" s="3" t="s">
         <x:v>9</x:v>
@@ -903,16 +1010,16 @@
     </x:row>
     <x:row r="22" spans="1:6">
       <x:c r="A22" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B22" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C22" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D22" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E22" s="3" t="s">
         <x:v>10</x:v>
@@ -921,13 +1028,13 @@
     </x:row>
     <x:row r="23" spans="1:6">
       <x:c r="A23" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B23" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C23" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D23" s="3" t="s">
         <x:v>9</x:v>
@@ -957,16 +1064,16 @@
     </x:row>
     <x:row r="25" spans="1:6">
       <x:c r="A25" s="3" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B25" s="3" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C25" s="3" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D25" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E25" s="3" t="s">
         <x:v>10</x:v>
@@ -975,13 +1082,13 @@
     </x:row>
     <x:row r="26" spans="1:6">
       <x:c r="A26" s="3" t="s">
-        <x:v>15</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="B26" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C26" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D26" s="3" t="s">
         <x:v>9</x:v>
@@ -993,16 +1100,16 @@
     </x:row>
     <x:row r="27" spans="1:6">
       <x:c r="A27" s="3" t="s">
-        <x:v>18</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="B27" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C27" s="3" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="D27" s="3" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E27" s="3" t="s">
         <x:v>10</x:v>
@@ -1011,13 +1118,13 @@
     </x:row>
     <x:row r="28" spans="1:6">
       <x:c r="A28" s="3" t="s">
-        <x:v>21</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B28" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C28" s="3" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D28" s="3" t="s">
         <x:v>9</x:v>
@@ -1029,13 +1136,13 @@
     </x:row>
     <x:row r="29" spans="1:6">
       <x:c r="A29" s="3" t="s">
-        <x:v>23</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B29" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C29" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D29" s="3" t="s">
         <x:v>9</x:v>
@@ -1047,13 +1154,13 @@
     </x:row>
     <x:row r="30" spans="1:6">
       <x:c r="A30" s="3" t="s">
-        <x:v>25</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B30" s="3" t="s">
-        <x:v>16</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C30" s="3" t="s">
-        <x:v>17</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="D30" s="3" t="s">
         <x:v>9</x:v>
@@ -1065,13 +1172,13 @@
     </x:row>
     <x:row r="31" spans="1:6">
       <x:c r="A31" s="3" t="s">
-        <x:v>26</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="B31" s="3" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C31" s="3" t="s">
         <x:v>19</x:v>
-      </x:c>
-      <x:c r="C31" s="3" t="s">
-        <x:v>17</x:v>
       </x:c>
       <x:c r="D31" s="3" t="s">
         <x:v>9</x:v>
@@ -1083,13 +1190,13 @@
     </x:row>
     <x:row r="32" spans="1:6">
       <x:c r="A32" s="3" t="s">
-        <x:v>27</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B32" s="3" t="s">
-        <x:v>19</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="C32" s="3" t="s">
-        <x:v>24</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D32" s="3" t="s">
         <x:v>9</x:v>
@@ -1101,18 +1208,234 @@
     </x:row>
     <x:row r="33" spans="1:6">
       <x:c r="A33" s="3" t="s">
-        <x:v>28</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B33" s="3" t="s">
-        <x:v>29</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C33" s="3" t="s">
-        <x:v>30</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D33" s="3" t="s">
         <x:v>9</x:v>
       </x:c>
       <x:c r="E33" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F33" s="3" t="s"/>
+    </x:row>
+    <x:row r="34" spans="1:6">
+      <x:c r="A34" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B34" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C34" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D34" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E34" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F34" s="3" t="s"/>
+    </x:row>
+    <x:row r="35" spans="1:6">
+      <x:c r="A35" s="3" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B35" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C35" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D35" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E35" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F35" s="3" t="s"/>
+    </x:row>
+    <x:row r="36" spans="1:6">
+      <x:c r="A36" s="3" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="B36" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C36" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D36" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E36" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F36" s="3" t="s"/>
+    </x:row>
+    <x:row r="37" spans="1:6">
+      <x:c r="A37" s="3" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B37" s="3" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C37" s="3" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D37" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E37" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F37" s="3" t="s"/>
+    </x:row>
+    <x:row r="38" spans="1:6">
+      <x:c r="A38" s="3" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B38" s="3" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C38" s="3" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D38" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E38" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F38" s="3" t="s"/>
+    </x:row>
+    <x:row r="39" spans="1:6">
+      <x:c r="A39" s="3" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="B39" s="3" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C39" s="3" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="D39" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E39" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F39" s="3" t="s"/>
+    </x:row>
+    <x:row r="40" spans="1:6">
+      <x:c r="A40" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B40" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="C40" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="D40" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E40" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F40" s="3" t="s"/>
+    </x:row>
+    <x:row r="41" spans="1:6">
+      <x:c r="A41" s="3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B41" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="C41" s="3" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D41" s="3" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E41" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F41" s="3" t="s"/>
+    </x:row>
+    <x:row r="42" spans="1:6">
+      <x:c r="A42" s="3" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B42" s="3" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C42" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D42" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E42" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F42" s="3" t="s"/>
+    </x:row>
+    <x:row r="43" spans="1:6">
+      <x:c r="A43" s="3" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="B43" s="3" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="C43" s="3" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D43" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E43" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F43" s="3" t="s"/>
+    </x:row>
+    <x:row r="44" spans="1:6">
+      <x:c r="A44" s="3" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="B44" s="3" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="C44" s="3" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D44" s="3" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E44" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F44" s="3" t="s"/>
+    </x:row>
+    <x:row r="45" spans="1:6">
+      <x:c r="A45" s="3" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B45" s="3" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="C45" s="3" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="D45" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="E45" s="3" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
FIxed duplication issue with UniqueJobs.
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Projects\P3SalesAutomationSuite\ScrapeJobPostData\CareerBuilderWorkflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\P3 Sales\P3SalesAutomationSuite\ScrapeJobPostData\CareerBuilderWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8448A811-1FBC-410F-8B34-2EEE115B3E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781DB155-CDAB-4FF6-B743-8525F46C86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="0" activeTab="0" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="CareerBuilder" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <x:t>N/A</x:t>
   </x:si>
   <x:si>
-    <x:t>718</x:t>
+    <x:t>696</x:t>
   </x:si>
   <x:si>
     <x:t>16 days ago</x:t>
@@ -133,7 +133,7 @@
     <x:t>Dallas, TX</x:t>
   </x:si>
   <x:si>
-    <x:t>2,025</x:t>
+    <x:t>1,955</x:t>
   </x:si>
   <x:si>
     <x:t>21 days ago</x:t>
@@ -163,34 +163,34 @@
     <x:t>https://www.careerbuilder.com/job/JD867K661MNLSH8N6XW</x:t>
   </x:si>
   <x:si>
+    <x:t>Facilities Engineer - Electrical - Entry/Experienced Level (NSAW and NSAH)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>National Security Agency (NSA)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Fort Meade, MD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12 days ago</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.careerbuilder.com/job/J3Q4ML75ZRJFH5DYB94</x:t>
+  </x:si>
+  <x:si>
     <x:t>Entry Level Marketing</x:t>
   </x:si>
   <x:si>
     <x:t>DFW Brands</x:t>
   </x:si>
   <x:si>
-    <x:t>1 day ago</x:t>
+    <x:t>2 days ago</x:t>
   </x:si>
   <x:si>
     <x:t>https://www.careerbuilder.com/job/J2W5L86NHXHH00GX3ZS</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Facilities Engineer - Electrical - Entry/Experienced Level (NSAW and NSAH)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>National Security Agency (NSA)</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Fort Meade, MD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>12 days ago</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.careerbuilder.com/job/J3Q4ML75ZRJFH5DYB94</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -562,10 +562,10 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:L5"/>
+  <x:dimension ref="A1:L1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <x:selection activeCell="L5" sqref="L5 L5:L5 A2:L5"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A2" sqref="A2 A2:A2 A2:C7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,8 @@
     <x:col min="7" max="7" width="23.285156" style="2" customWidth="1"/>
     <x:col min="8" max="8" width="19.425781" style="2" customWidth="1"/>
     <x:col min="9" max="9" width="17.570312" style="2" customWidth="1"/>
-    <x:col min="10" max="11" width="9.140625" style="2" customWidth="1"/>
+    <x:col min="10" max="10" width="9.140625" style="2" customWidth="1"/>
+    <x:col min="11" max="11" width="13.425781" style="2" bestFit="1" customWidth="1"/>
     <x:col min="12" max="12" width="57.140625" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -621,7 +622,7 @@
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <x:row r="2" spans="1:12">
       <x:c r="A2" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -659,7 +660,7 @@
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <x:row r="3" spans="1:12">
       <x:c r="A3" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -678,7 +679,6 @@
       <x:c r="F3" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="G3" s="2" t="s"/>
       <x:c r="H3" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -695,7 +695,7 @@
         <x:v>28</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <x:row r="4" spans="1:12">
       <x:c r="A4" s="2" t="s">
         <x:v>12</x:v>
       </x:c>
@@ -733,7 +733,7 @@
         <x:v>34</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <x:row r="5" spans="1:12">
       <x:c r="A5" s="2" t="s">
         <x:v>35</x:v>
       </x:c>
@@ -752,7 +752,6 @@
       <x:c r="F5" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="G5" s="2" t="s"/>
       <x:c r="H5" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
@@ -780,7 +779,7 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
-        <x:v>31</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E6" s="2" t="s">
         <x:v>16</x:v>
@@ -788,8 +787,11 @@
       <x:c r="F6" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="G6" s="2" t="s">
+        <x:v>45</x:v>
+      </x:c>
       <x:c r="H6" s="2" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="I6" s="2" t="s">
         <x:v>20</x:v>
@@ -801,7 +803,7 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="L6" s="2" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:12">
@@ -809,22 +811,19 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="B7" s="2" t="s">
-        <x:v>46</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C7" s="2" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D7" s="2" t="s">
-        <x:v>48</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E7" s="2" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="F7" s="2" t="s">
         <x:v>17</x:v>
-      </x:c>
-      <x:c r="G7" s="2" t="s">
-        <x:v>49</x:v>
       </x:c>
       <x:c r="H7" s="2" t="s">
         <x:v>50</x:v>

</xml_diff>

<commit_message>
Fixed Unique Jobs not printing. Added Assign and Write Cell activities to If CompanySize Else statement.
</commit_message>
<xml_diff>
--- a/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
+++ b/ScrapeJobPostData/CareerBuilderWorkflow/CBExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Programming\Revature\Revature UIPath Batch\P3 Sales\P3SalesAutomationSuite\ScrapeJobPostData\CareerBuilderWorkflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781DB155-CDAB-4FF6-B743-8525F46C86A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0CC592-812D-4FA9-B248-DF848698EEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{3392AAAF-4571-4630-9A5F-84526169A893}"/>
   </x:bookViews>
@@ -564,8 +564,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:L1"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A2" sqref="A2 A2:A2 A2:C7"/>
+    <x:sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <x:selection activeCell="A2" sqref="A2 A2:A2 A2:L7 A2:C7"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +679,9 @@
       <x:c r="F3" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="G3" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
       <x:c r="H3" s="2" t="s">
         <x:v>27</x:v>
       </x:c>
@@ -752,6 +755,9 @@
       <x:c r="F5" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
+      <x:c r="G5" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
       <x:c r="H5" s="2" t="s">
         <x:v>40</x:v>
       </x:c>
@@ -823,6 +829,9 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="F7" s="2" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="G7" s="2" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="H7" s="2" t="s">

</xml_diff>